<commit_message>
Unify and balance the data
</commit_message>
<xml_diff>
--- a/Carbon Emission Factor Database.xlsx
+++ b/Carbon Emission Factor Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxinyi/Desktop/InteractiveDB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A924DC7-5D3B-6C41-89AB-8B80BF518DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02EC4D0-7FFB-4444-9270-F78CE3D96E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13297,8 +13297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313F4BBB-8598-4D33-B468-165E95491FC7}">
   <dimension ref="A1:S425"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13362,7 +13362,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17">
+    <row r="2" spans="1:14" ht="18">
       <c r="A2" s="3" t="s">
         <v>1221</v>
       </c>
@@ -13376,10 +13376,10 @@
         <v>3.15</v>
       </c>
       <c r="E2" s="3">
-        <v>735</v>
+        <v>2315.25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -13400,7 +13400,7 @@
       </c>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="17">
+    <row r="3" spans="1:14" ht="18">
       <c r="A3" s="3" t="s">
         <v>1049</v>
       </c>
@@ -13414,10 +13414,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E3" s="3">
-        <v>295</v>
+        <v>678.5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -13438,7 +13438,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="17">
+    <row r="4" spans="1:14" ht="18">
       <c r="A4" s="3" t="s">
         <v>1050</v>
       </c>
@@ -13452,10 +13452,10 @@
         <v>2.4</v>
       </c>
       <c r="E4" s="3">
-        <v>385</v>
+        <v>924</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -13476,7 +13476,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="17">
+    <row r="5" spans="1:14" ht="18">
       <c r="A5" s="3" t="s">
         <v>1051</v>
       </c>
@@ -13493,7 +13493,7 @@
         <v>1190</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -13514,7 +13514,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="17">
+    <row r="6" spans="1:14" ht="18">
       <c r="A6" s="3" t="s">
         <v>1048</v>
       </c>
@@ -13528,10 +13528,10 @@
         <v>2.21</v>
       </c>
       <c r="E6" s="3">
-        <v>747</v>
+        <v>2975</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -13552,7 +13552,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="17">
+    <row r="7" spans="1:14" ht="18">
       <c r="A7" s="3" t="s">
         <v>1052</v>
       </c>
@@ -13566,10 +13566,10 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="E7" s="3">
-        <v>32.799999999999997</v>
+        <v>83.64</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -13590,7 +13590,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="17">
+    <row r="8" spans="1:14" ht="18">
       <c r="A8" s="3" t="s">
         <v>1047</v>
       </c>
@@ -13604,10 +13604,10 @@
         <v>1.5</v>
       </c>
       <c r="E8" s="3">
-        <v>2.5099999999999998</v>
+        <v>3.7650000000000001</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -13628,7 +13628,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="17">
+    <row r="9" spans="1:14" ht="18">
       <c r="A9" s="3" t="s">
         <v>1046</v>
       </c>
@@ -13642,10 +13642,10 @@
         <v>1.75</v>
       </c>
       <c r="E9" s="3">
-        <v>2.1800000000000002</v>
+        <v>3.8149999999999999</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -13666,7 +13666,7 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="17">
+    <row r="10" spans="1:14" ht="18">
       <c r="A10" s="3" t="s">
         <v>1053</v>
       </c>
@@ -13680,10 +13680,10 @@
         <v>2.8</v>
       </c>
       <c r="E10" s="3">
-        <v>5.08</v>
+        <v>14.224</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -13704,7 +13704,7 @@
       </c>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" ht="17">
+    <row r="11" spans="1:14" ht="18">
       <c r="A11" s="3" t="s">
         <v>1054</v>
       </c>
@@ -13718,10 +13718,10 @@
         <v>2.1</v>
       </c>
       <c r="E11" s="3">
-        <v>2.69</v>
+        <v>5.649</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>998</v>
+        <v>1003</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>

</xml_diff>